<commit_message>
[DESC]: Add modifications to enter/exit from production test mode
</commit_message>
<xml_diff>
--- a/r1_test_command_list_tag1.1.xlsx
+++ b/r1_test_command_list_tag1.1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="199">
   <si>
     <t>./inventory.sh</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -360,10 +360,6 @@
 </t>
   </si>
   <si>
-    <t>Record Failed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Set MAC Address Failed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -538,9 +534,6 @@
     </r>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -722,6 +715,9 @@
   </si>
   <si>
     <t>Added. Recorded mic track is in here: /data/factory-test/mic-4ch.wav</t>
+  </si>
+  <si>
+    <t>Record Failed</t>
   </si>
 </sst>
 </file>
@@ -820,7 +816,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -854,12 +850,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -928,7 +918,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -981,15 +971,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -999,7 +980,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1020,7 +1001,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1329,14 +1310,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.85546875" style="14" customWidth="1"/>
-    <col min="2" max="2" width="6" style="25" customWidth="1"/>
+    <col min="2" max="2" width="6" style="22" customWidth="1"/>
     <col min="3" max="3" width="37" style="14" customWidth="1"/>
     <col min="4" max="4" width="46.5703125" style="14" customWidth="1"/>
     <col min="5" max="5" width="46.7109375" style="14" customWidth="1"/>
@@ -1347,7 +1328,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="27" customHeight="1">
       <c r="A1" s="15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>19</v>
@@ -1362,45 +1343,49 @@
         <v>18</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1">
-      <c r="A2" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="B2" s="22"/>
+      <c r="A2" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="25">
+        <v>1</v>
+      </c>
       <c r="C2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="23" t="s">
         <v>88</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G2" s="18"/>
       <c r="H2" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="45" customHeight="1">
-      <c r="A3" s="29"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="25">
+        <v>2</v>
+      </c>
       <c r="C3" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>141</v>
+        <v>153</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>139</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>15</v>
@@ -1410,55 +1395,61 @@
       </c>
       <c r="G3" s="18"/>
       <c r="H3" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="29"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="25">
+        <v>3</v>
+      </c>
       <c r="C4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="24" t="s">
         <v>86</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F4" s="18" t="s">
         <v>92</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
-      <c r="A5" s="29"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="25">
+        <v>4</v>
+      </c>
       <c r="C5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="24" t="s">
         <v>87</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F5" s="18"/>
       <c r="G5" s="18"/>
       <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="29"/>
-      <c r="B6" s="22"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="25">
+        <v>5</v>
+      </c>
       <c r="C6" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>153</v>
+        <v>150</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>151</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>9</v>
@@ -1468,12 +1459,14 @@
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1">
-      <c r="A7" s="29"/>
-      <c r="B7" s="22"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="25">
+        <v>6</v>
+      </c>
       <c r="C7" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="23" t="s">
         <v>85</v>
       </c>
       <c r="E7" s="17" t="s">
@@ -1484,28 +1477,32 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1">
-      <c r="A8" s="29"/>
-      <c r="B8" s="22"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="25">
+        <v>7</v>
+      </c>
       <c r="C8" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>154</v>
+        <v>149</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>152</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1">
-      <c r="A9" s="29"/>
-      <c r="B9" s="22"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="25">
+        <v>8</v>
+      </c>
       <c r="C9" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="24" t="s">
         <v>90</v>
       </c>
       <c r="E9" s="18" t="s">
@@ -1515,57 +1512,63 @@
       <c r="G9" s="18"/>
       <c r="H9" s="10"/>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1">
-      <c r="A10" s="29"/>
-      <c r="B10" s="22"/>
+    <row r="10" spans="1:8" ht="56.25" customHeight="1">
+      <c r="A10" s="26"/>
+      <c r="B10" s="25">
+        <v>9</v>
+      </c>
       <c r="C10" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>140</v>
+        <v>135</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>138</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>13</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>97</v>
+        <v>198</v>
       </c>
       <c r="G10" s="18" t="s">
         <v>95</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1">
-      <c r="A11" s="29"/>
-      <c r="B11" s="22"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="25">
+        <v>10</v>
+      </c>
       <c r="C11" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>149</v>
+        <v>155</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>147</v>
       </c>
       <c r="E11" s="18" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G11" s="17" t="s">
         <v>96</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1">
-      <c r="A12" s="29"/>
-      <c r="B12" s="22"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="25">
+        <v>11</v>
+      </c>
       <c r="C12" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="24" t="s">
         <v>84</v>
       </c>
       <c r="E12" s="18" t="s">
@@ -1576,16 +1579,18 @@
       </c>
       <c r="G12" s="18"/>
       <c r="H12" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1">
-      <c r="A13" s="29"/>
-      <c r="B13" s="22"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="25">
+        <v>12</v>
+      </c>
       <c r="C13" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="27" t="s">
+      <c r="D13" s="24" t="s">
         <v>93</v>
       </c>
       <c r="E13" s="18" t="s">
@@ -1598,13 +1603,15 @@
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1">
-      <c r="A14" s="29"/>
-      <c r="B14" s="22"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="25">
+        <v>13</v>
+      </c>
       <c r="C14" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="D14" s="26" t="s">
-        <v>150</v>
+        <v>154</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>148</v>
       </c>
       <c r="E14" s="17" t="s">
         <v>10</v>
@@ -1614,475 +1621,515 @@
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1">
-      <c r="A15" s="29"/>
-      <c r="B15" s="22"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="25">
+        <v>14</v>
+      </c>
       <c r="C15" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="D15" s="26" t="s">
-        <v>160</v>
+        <v>157</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>158</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F15" s="18"/>
       <c r="G15" s="18"/>
       <c r="H15" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1">
-      <c r="A16" s="29"/>
-      <c r="B16" s="23" t="s">
-        <v>138</v>
+      <c r="A16" s="26"/>
+      <c r="B16" s="25">
+        <v>15</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="D16" s="26"/>
+        <v>99</v>
+      </c>
+      <c r="D16" s="23"/>
       <c r="E16" s="17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F16" s="18"/>
       <c r="G16" s="18"/>
       <c r="H16" s="12"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1">
-      <c r="A17" s="29"/>
-      <c r="B17" s="23" t="s">
-        <v>138</v>
+      <c r="A17" s="26"/>
+      <c r="B17" s="25">
+        <v>16</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="D17" s="26"/>
+        <v>100</v>
+      </c>
+      <c r="D17" s="23"/>
       <c r="E17" s="17" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
       <c r="H17" s="12"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1">
-      <c r="A18" s="29"/>
-      <c r="B18" s="23" t="s">
-        <v>138</v>
+      <c r="A18" s="26"/>
+      <c r="B18" s="25">
+        <v>17</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>167</v>
-      </c>
-      <c r="D18" s="26"/>
+        <v>165</v>
+      </c>
+      <c r="D18" s="23"/>
       <c r="E18" s="17" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F18" s="18"/>
       <c r="G18" s="18"/>
       <c r="H18" s="12"/>
     </row>
     <row r="19" spans="1:8" ht="15" customHeight="1">
-      <c r="A19" s="29"/>
-      <c r="B19" s="23" t="s">
-        <v>138</v>
+      <c r="A19" s="26"/>
+      <c r="B19" s="25">
+        <v>18</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="D19" s="26"/>
+        <v>162</v>
+      </c>
+      <c r="D19" s="23"/>
       <c r="E19" s="17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="18"/>
-      <c r="H19" s="12"/>
+      <c r="H19" s="10" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1">
-      <c r="A20" s="29"/>
-      <c r="B20" s="23" t="s">
-        <v>138</v>
+      <c r="A20" s="26"/>
+      <c r="B20" s="25">
+        <v>19</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="D20" s="26"/>
+        <v>101</v>
+      </c>
+      <c r="D20" s="23"/>
       <c r="E20" s="17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F20" s="18"/>
       <c r="G20" s="18"/>
-      <c r="H20" s="12"/>
+      <c r="H20" s="10" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1">
-      <c r="A21" s="29"/>
-      <c r="B21" s="28"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="25">
+        <v>20</v>
+      </c>
       <c r="C21" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="D21" s="26"/>
+        <v>102</v>
+      </c>
+      <c r="D21" s="23"/>
       <c r="E21" s="17" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
       <c r="H21" s="12"/>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1">
-      <c r="A22" s="29"/>
-      <c r="B22" s="28"/>
+      <c r="A22" s="26"/>
+      <c r="B22" s="25">
+        <v>21</v>
+      </c>
       <c r="C22" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="D22" s="26"/>
+        <v>103</v>
+      </c>
+      <c r="D22" s="23"/>
       <c r="E22" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F22" s="18"/>
       <c r="G22" s="18"/>
       <c r="H22" s="12"/>
     </row>
     <row r="23" spans="1:8" ht="15" customHeight="1">
-      <c r="A23" s="29"/>
-      <c r="B23" s="28"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="25">
+        <v>22</v>
+      </c>
       <c r="C23" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="D23" s="26"/>
+        <v>104</v>
+      </c>
+      <c r="D23" s="23"/>
       <c r="E23" s="17" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F23" s="18"/>
       <c r="G23" s="18"/>
       <c r="H23" s="12"/>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1">
-      <c r="A24" s="29"/>
-      <c r="B24" s="28"/>
+      <c r="A24" s="26"/>
+      <c r="B24" s="25">
+        <v>23</v>
+      </c>
       <c r="C24" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="D24" s="26"/>
+        <v>105</v>
+      </c>
+      <c r="D24" s="23"/>
       <c r="E24" s="17" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F24" s="18"/>
       <c r="G24" s="18"/>
       <c r="H24" s="12"/>
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1">
-      <c r="A25" s="29"/>
-      <c r="B25" s="28"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="25">
+        <v>24</v>
+      </c>
       <c r="C25" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="D25" s="26"/>
+        <v>106</v>
+      </c>
+      <c r="D25" s="23"/>
       <c r="E25" s="17" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F25" s="18"/>
       <c r="G25" s="18"/>
       <c r="H25" s="12"/>
     </row>
     <row r="26" spans="1:8" ht="15" customHeight="1">
-      <c r="A26" s="29"/>
-      <c r="B26" s="28"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="25">
+        <v>25</v>
+      </c>
       <c r="C26" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="D26" s="26"/>
+        <v>107</v>
+      </c>
+      <c r="D26" s="23"/>
       <c r="E26" s="17" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F26" s="18"/>
       <c r="G26" s="18"/>
       <c r="H26" s="12"/>
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1">
-      <c r="A27" s="29"/>
-      <c r="B27" s="28"/>
+      <c r="A27" s="26"/>
+      <c r="B27" s="25">
+        <v>26</v>
+      </c>
       <c r="C27" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="D27" s="26"/>
+        <v>108</v>
+      </c>
+      <c r="D27" s="23"/>
       <c r="E27" s="17" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F27" s="18"/>
       <c r="G27" s="18"/>
       <c r="H27" s="12"/>
     </row>
     <row r="28" spans="1:8" ht="15" customHeight="1">
-      <c r="A28" s="29"/>
-      <c r="B28" s="28"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="25">
+        <v>27</v>
+      </c>
       <c r="C28" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="D28" s="26"/>
+        <v>109</v>
+      </c>
+      <c r="D28" s="23"/>
       <c r="E28" s="17" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F28" s="18"/>
       <c r="G28" s="18"/>
       <c r="H28" s="12"/>
     </row>
     <row r="29" spans="1:8" ht="15" customHeight="1">
-      <c r="A29" s="29"/>
-      <c r="B29" s="28"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="25">
+        <v>28</v>
+      </c>
       <c r="C29" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="D29" s="26"/>
+        <v>110</v>
+      </c>
+      <c r="D29" s="23"/>
       <c r="E29" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F29" s="18"/>
       <c r="G29" s="18"/>
       <c r="H29" s="12"/>
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1">
-      <c r="A30" s="29"/>
-      <c r="B30" s="22"/>
+      <c r="A30" s="26"/>
+      <c r="B30" s="25">
+        <v>29</v>
+      </c>
       <c r="C30" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="D30" s="26" t="s">
         <v>163</v>
       </c>
+      <c r="D30" s="23" t="s">
+        <v>161</v>
+      </c>
       <c r="E30" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F30" s="18"/>
       <c r="G30" s="18"/>
       <c r="H30" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1">
-      <c r="A31" s="29"/>
-      <c r="B31" s="28"/>
+      <c r="A31" s="26"/>
+      <c r="B31" s="25">
+        <v>30</v>
+      </c>
       <c r="C31" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="D31" s="26"/>
+        <v>129</v>
+      </c>
+      <c r="D31" s="23"/>
       <c r="E31" s="17" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F31" s="18"/>
       <c r="G31" s="18"/>
       <c r="H31" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15" customHeight="1">
-      <c r="A32" s="29"/>
-      <c r="B32" s="28"/>
+      <c r="A32" s="26"/>
+      <c r="B32" s="25">
+        <v>31</v>
+      </c>
       <c r="C32" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="D32" s="26"/>
+        <v>112</v>
+      </c>
+      <c r="D32" s="23"/>
       <c r="E32" s="17" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F32" s="18"/>
       <c r="G32" s="18"/>
       <c r="H32" s="12"/>
     </row>
     <row r="33" spans="1:8" ht="15" customHeight="1">
-      <c r="A33" s="29"/>
-      <c r="B33" s="22"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="25">
+        <v>32</v>
+      </c>
       <c r="C33" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="D33" s="26" t="s">
-        <v>161</v>
+        <v>164</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>159</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F33" s="18"/>
       <c r="G33" s="18"/>
       <c r="H33" s="10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15" customHeight="1">
+      <c r="A34" s="26"/>
+      <c r="B34" s="25">
+        <v>33</v>
+      </c>
+      <c r="C34" s="21" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="15" customHeight="1">
-      <c r="A34" s="29"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="D34" s="26" t="s">
-        <v>162</v>
+      <c r="D34" s="23" t="s">
+        <v>160</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F34" s="18"/>
       <c r="G34" s="18"/>
       <c r="H34" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15" customHeight="1">
-      <c r="A35" s="29"/>
-      <c r="B35" s="23" t="s">
-        <v>138</v>
+      <c r="A35" s="26"/>
+      <c r="B35" s="25">
+        <v>34</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="D35" s="26"/>
+        <v>113</v>
+      </c>
+      <c r="D35" s="23"/>
       <c r="E35" s="17" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F35" s="18"/>
       <c r="G35" s="18"/>
       <c r="H35" s="12"/>
     </row>
     <row r="36" spans="1:8" ht="15" customHeight="1">
-      <c r="A36" s="29"/>
-      <c r="B36" s="23" t="s">
-        <v>138</v>
+      <c r="A36" s="26"/>
+      <c r="B36" s="25">
+        <v>35</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="D36" s="26"/>
+        <v>114</v>
+      </c>
+      <c r="D36" s="23"/>
       <c r="E36" s="17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F36" s="18"/>
       <c r="G36" s="18"/>
       <c r="H36" s="12"/>
     </row>
     <row r="37" spans="1:8" ht="15" customHeight="1">
-      <c r="A37" s="29"/>
-      <c r="B37" s="28"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="25">
+        <v>36</v>
+      </c>
       <c r="C37" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="D37" s="26"/>
+        <v>115</v>
+      </c>
+      <c r="D37" s="23"/>
       <c r="E37" s="17" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F37" s="18"/>
       <c r="G37" s="18"/>
       <c r="H37" s="12"/>
     </row>
     <row r="38" spans="1:8" ht="15" customHeight="1">
-      <c r="A38" s="29"/>
-      <c r="B38" s="28"/>
+      <c r="A38" s="26"/>
+      <c r="B38" s="25">
+        <v>37</v>
+      </c>
       <c r="C38" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="D38" s="26"/>
+        <v>116</v>
+      </c>
+      <c r="D38" s="23"/>
       <c r="E38" s="17" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F38" s="18"/>
       <c r="G38" s="18"/>
       <c r="H38" s="12"/>
     </row>
     <row r="39" spans="1:8" ht="15" customHeight="1">
-      <c r="A39" s="29"/>
-      <c r="B39" s="28"/>
+      <c r="A39" s="26"/>
+      <c r="B39" s="25">
+        <v>38</v>
+      </c>
       <c r="C39" s="21" t="s">
-        <v>118</v>
-      </c>
-      <c r="D39" s="26"/>
+        <v>117</v>
+      </c>
+      <c r="D39" s="23"/>
       <c r="E39" s="17" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F39" s="18"/>
       <c r="G39" s="18"/>
       <c r="H39" s="12"/>
     </row>
     <row r="40" spans="1:8" ht="15" customHeight="1">
-      <c r="A40" s="29"/>
-      <c r="B40" s="35" t="s">
-        <v>138</v>
+      <c r="A40" s="26"/>
+      <c r="B40" s="25">
+        <v>39</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="D40" s="27"/>
+        <v>118</v>
+      </c>
+      <c r="D40" s="24"/>
       <c r="E40" s="17" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F40" s="18"/>
       <c r="G40" s="18"/>
       <c r="H40" s="12"/>
     </row>
     <row r="41" spans="1:8" ht="15" customHeight="1">
-      <c r="A41" s="29"/>
-      <c r="B41" s="35" t="s">
-        <v>138</v>
+      <c r="A41" s="26"/>
+      <c r="B41" s="25">
+        <v>40</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="D41" s="27"/>
+        <v>119</v>
+      </c>
+      <c r="D41" s="24"/>
       <c r="E41" s="17" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F41" s="18"/>
       <c r="G41" s="18"/>
       <c r="H41" s="12"/>
     </row>
     <row r="42" spans="1:8" ht="15" customHeight="1">
-      <c r="A42" s="29"/>
-      <c r="B42" s="35" t="s">
-        <v>138</v>
+      <c r="A42" s="26"/>
+      <c r="B42" s="25">
+        <v>41</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="D42" s="27"/>
+        <v>120</v>
+      </c>
+      <c r="D42" s="24"/>
       <c r="E42" s="17" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F42" s="18"/>
       <c r="G42" s="18"/>
       <c r="H42" s="12"/>
     </row>
     <row r="43" spans="1:8" ht="15" customHeight="1">
-      <c r="A43" s="29" t="s">
-        <v>134</v>
-      </c>
-      <c r="B43" s="24">
+      <c r="A43" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="B43" s="32">
         <v>1</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>197</v>
-      </c>
-      <c r="D43" s="27" t="s">
-        <v>131</v>
+        <v>195</v>
+      </c>
+      <c r="D43" s="24" t="s">
+        <v>130</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F43" s="18"/>
       <c r="G43" s="18"/>
       <c r="H43" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15" customHeight="1">
-      <c r="A44" s="29"/>
-      <c r="B44" s="24">
+      <c r="A44" s="26"/>
+      <c r="B44" s="32">
         <v>2</v>
       </c>
       <c r="C44" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="D44" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="D44" s="27" t="s">
-        <v>133</v>
-      </c>
       <c r="E44" s="18" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F44" s="18"/>
       <c r="G44" s="18"/>
       <c r="H44" s="10" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="49" spans="4:4">
@@ -2119,7 +2166,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="31" t="s">
         <v>75</v>
       </c>
       <c r="B1" s="8" t="s">
@@ -2127,19 +2174,19 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="34"/>
+      <c r="A2" s="31"/>
       <c r="B2" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="34"/>
+      <c r="A3" s="31"/>
       <c r="B3" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="31" t="s">
         <v>76</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -2147,19 +2194,19 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="34"/>
+      <c r="A5" s="31"/>
       <c r="B5" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="34"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="31" t="s">
         <v>74</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -2167,19 +2214,19 @@
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="34"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="34"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="31" t="s">
         <v>77</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -2187,19 +2234,19 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="34"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="7" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="34"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="6" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="31" t="s">
         <v>73</v>
       </c>
       <c r="B13" s="8" t="s">
@@ -2207,19 +2254,19 @@
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="34"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="7" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="34"/>
+      <c r="A15" s="31"/>
       <c r="B15" s="6" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="30" t="s">
         <v>78</v>
       </c>
       <c r="B16" s="8" t="s">
@@ -2227,19 +2274,19 @@
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="33"/>
+      <c r="A17" s="30"/>
       <c r="B17" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="33"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="6" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="30" t="s">
         <v>79</v>
       </c>
       <c r="B19" s="8" t="s">
@@ -2247,250 +2294,250 @@
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="33"/>
+      <c r="A20" s="30"/>
       <c r="B20" s="7" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="33"/>
+      <c r="A21" s="30"/>
       <c r="B21" s="6" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="30" t="s">
         <v>72</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="30" t="s">
+      <c r="C22" s="27" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="33"/>
+      <c r="A23" s="30"/>
       <c r="B23" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="31"/>
+      <c r="C23" s="28"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="33"/>
+      <c r="A24" s="30"/>
       <c r="B24" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="31"/>
+      <c r="C24" s="28"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="33"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="31"/>
+      <c r="C25" s="28"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="33"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="31"/>
+      <c r="C26" s="28"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="33"/>
+      <c r="A27" s="30"/>
       <c r="B27" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="31"/>
+      <c r="C27" s="28"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="33"/>
+      <c r="A28" s="30"/>
       <c r="B28" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="31"/>
+      <c r="C28" s="28"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="33"/>
+      <c r="A29" s="30"/>
       <c r="B29" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="31"/>
+      <c r="C29" s="28"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="30" t="s">
         <v>80</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="31"/>
+      <c r="C30" s="28"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="33"/>
+      <c r="A31" s="30"/>
       <c r="B31" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="31"/>
+      <c r="C31" s="28"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="33"/>
+      <c r="A32" s="30"/>
       <c r="B32" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="31"/>
+      <c r="C32" s="28"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="33"/>
+      <c r="A33" s="30"/>
       <c r="B33" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="31"/>
+      <c r="C33" s="28"/>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="33"/>
+      <c r="A34" s="30"/>
       <c r="B34" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="31"/>
+      <c r="C34" s="28"/>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="33"/>
+      <c r="A35" s="30"/>
       <c r="B35" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="31"/>
+      <c r="C35" s="28"/>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="33"/>
+      <c r="A36" s="30"/>
       <c r="B36" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C36" s="31"/>
+      <c r="C36" s="28"/>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="33"/>
+      <c r="A37" s="30"/>
       <c r="B37" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C37" s="31"/>
+      <c r="C37" s="28"/>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="33" t="s">
+      <c r="A38" s="30" t="s">
         <v>81</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="31"/>
+      <c r="C38" s="28"/>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="33"/>
+      <c r="A39" s="30"/>
       <c r="B39" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="31"/>
+      <c r="C39" s="28"/>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="33"/>
+      <c r="A40" s="30"/>
       <c r="B40" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="31"/>
+      <c r="C40" s="28"/>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="33"/>
+      <c r="A41" s="30"/>
       <c r="B41" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="31"/>
+      <c r="C41" s="28"/>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="33"/>
+      <c r="A42" s="30"/>
       <c r="B42" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C42" s="31"/>
+      <c r="C42" s="28"/>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="33"/>
+      <c r="A43" s="30"/>
       <c r="B43" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C43" s="31"/>
+      <c r="C43" s="28"/>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="33"/>
+      <c r="A44" s="30"/>
       <c r="B44" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="31"/>
+      <c r="C44" s="28"/>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="33"/>
+      <c r="A45" s="30"/>
       <c r="B45" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="31"/>
+      <c r="C45" s="28"/>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="33" t="s">
+      <c r="A46" s="30" t="s">
         <v>82</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C46" s="31"/>
+      <c r="C46" s="28"/>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="33"/>
+      <c r="A47" s="30"/>
       <c r="B47" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C47" s="31"/>
+      <c r="C47" s="28"/>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="33"/>
+      <c r="A48" s="30"/>
       <c r="B48" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C48" s="31"/>
+      <c r="C48" s="28"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="33"/>
+      <c r="A49" s="30"/>
       <c r="B49" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C49" s="31"/>
+      <c r="C49" s="28"/>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="33"/>
+      <c r="A50" s="30"/>
       <c r="B50" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C50" s="31"/>
+      <c r="C50" s="28"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="33"/>
+      <c r="A51" s="30"/>
       <c r="B51" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C51" s="31"/>
+      <c r="C51" s="28"/>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="33"/>
+      <c r="A52" s="30"/>
       <c r="B52" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C52" s="31"/>
+      <c r="C52" s="28"/>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="33"/>
+      <c r="A53" s="30"/>
       <c r="B53" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C53" s="32"/>
+      <c r="C53" s="29"/>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="9"/>

</xml_diff>